<commit_message>
Early web interface components
</commit_message>
<xml_diff>
--- a/_reference/Soviet OOBs.xlsx
+++ b/_reference/Soviet OOBs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2760" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2760" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="2" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="SAM (SA6)" sheetId="7" r:id="rId7"/>
     <sheet name="SAM (SA8)" sheetId="8" r:id="rId8"/>
     <sheet name="AA Bde" sheetId="9" r:id="rId9"/>
+    <sheet name="Recce Btn" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="133">
   <si>
     <t>MRR</t>
   </si>
@@ -428,6 +429,15 @@
   </si>
   <si>
     <t>1985 soviets had 1900 T-80s in Europe</t>
+  </si>
+  <si>
+    <t>Personnel ea</t>
+  </si>
+  <si>
+    <t>Recce Battalion</t>
+  </si>
+  <si>
+    <t>Ural 375 POL</t>
   </si>
 </sst>
 </file>
@@ -438,7 +448,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -455,6 +465,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -494,7 +512,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -518,6 +536,16 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="60" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="60" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="60" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -845,7 +873,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,6 +957,396 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="9" width="6.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="9">
+        <f>SUM(D2:P2)</f>
+        <v>285</v>
+      </c>
+      <c r="D2" s="3">
+        <f>SUMPRODUCT(D3:D54,$B$3:$B$54)</f>
+        <v>285</v>
+      </c>
+      <c r="E2" s="3">
+        <f t="shared" ref="E2:J2" si="0">SUMPRODUCT(E3:E54,$B$3:$B$54)</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J2" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K2" s="3">
+        <f>SUMPRODUCT(K3:K54,$B$3:$B$54)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="14">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9">
+        <f t="shared" ref="C3:C16" si="1">SUM(D3:P3)</f>
+        <v>13</v>
+      </c>
+      <c r="D3" s="3">
+        <v>13</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="14">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="D4" s="3">
+        <v>25</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="14">
+        <v>1</v>
+      </c>
+      <c r="C5" s="9">
+        <f t="shared" si="1"/>
+        <v>122</v>
+      </c>
+      <c r="D5">
+        <v>122</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="14">
+        <v>2</v>
+      </c>
+      <c r="C6" s="9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="14">
+        <v>2</v>
+      </c>
+      <c r="C7" s="9">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="14">
+        <v>2</v>
+      </c>
+      <c r="C8" s="9">
+        <f>SUM(D8:P8)</f>
+        <v>3</v>
+      </c>
+      <c r="D8" s="3">
+        <v>3</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="14">
+        <v>2</v>
+      </c>
+      <c r="C9" s="9">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="D9" s="3">
+        <v>12</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="14">
+        <v>3</v>
+      </c>
+      <c r="C10" s="9">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="D10" s="3">
+        <v>6</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="14">
+        <v>2</v>
+      </c>
+      <c r="C11" s="9">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="D11" s="3">
+        <v>6</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="14">
+        <v>2</v>
+      </c>
+      <c r="C12" s="9">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D12" s="3">
+        <v>5</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="14">
+        <v>1</v>
+      </c>
+      <c r="C13" s="9">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="D13" s="3">
+        <f>2+4+13</f>
+        <v>19</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="9">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="D14" s="3">
+        <v>17</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="14">
+        <v>1</v>
+      </c>
+      <c r="C15" s="9">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="D15" s="3">
+        <v>11</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B16" s="14">
+        <v>1</v>
+      </c>
+      <c r="C16" s="9">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="D16" s="3">
+        <v>2</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="9"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="9"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -937,10 +1355,10 @@
   <dimension ref="A1:O99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3:B33"/>
+      <selection pane="bottomRight" activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3267,10 +3685,10 @@
   <dimension ref="A1:O96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B22" sqref="B22:B30"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5525,10 +5943,10 @@
   <dimension ref="A1:M55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B24" sqref="B24:B27"/>
+      <selection pane="bottomRight" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6910,7 +7328,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7555,7 +7973,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A3" sqref="A3:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8211,8 +8629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8594,7 +9012,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15:E16"/>
+      <selection sqref="A1:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added more web def data
</commit_message>
<xml_diff>
--- a/_reference/Soviet OOBs.xlsx
+++ b/_reference/Soviet OOBs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2760" firstSheet="6" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2760" firstSheet="7" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,8 @@
     <sheet name="SAM (SA8)" sheetId="8" r:id="rId8"/>
     <sheet name="AA Bde" sheetId="9" r:id="rId9"/>
     <sheet name="Recce Btn" sheetId="10" r:id="rId10"/>
-    <sheet name="9 TD" sheetId="11" r:id="rId11"/>
+    <sheet name="TD" sheetId="11" r:id="rId11"/>
+    <sheet name="MRD" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="178">
   <si>
     <t>MRR</t>
   </si>
@@ -523,6 +524,57 @@
   </si>
   <si>
     <t xml:space="preserve">: </t>
+  </si>
+  <si>
+    <t>Motor Rifle Division</t>
+  </si>
+  <si>
+    <t>HQ</t>
+  </si>
+  <si>
+    <t>SAM regiment</t>
+  </si>
+  <si>
+    <t>SSM btn</t>
+  </si>
+  <si>
+    <t>AT btn</t>
+  </si>
+  <si>
+    <t>Recce Btn</t>
+  </si>
+  <si>
+    <t>Eng btn</t>
+  </si>
+  <si>
+    <t>Signal btn</t>
+  </si>
+  <si>
+    <t>Mat'l support btn</t>
+  </si>
+  <si>
+    <t>Maintenance btn</t>
+  </si>
+  <si>
+    <t>chemical protection o</t>
+  </si>
+  <si>
+    <t>Medical btn</t>
+  </si>
+  <si>
+    <t>MT-12</t>
+  </si>
+  <si>
+    <t>Mi-24 Hind</t>
+  </si>
+  <si>
+    <t>Mi-8T Hip C/Mi-17</t>
+  </si>
+  <si>
+    <t>Mi-8T Hip D/G</t>
+  </si>
+  <si>
+    <t>BMP-1/2</t>
   </si>
 </sst>
 </file>
@@ -1053,7 +1105,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K16"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1442,11 +1494,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I4" sqref="I4"/>
+      <selection pane="bottomRight" activeCell="J19" sqref="J19:M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2781,6 +2833,1010 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="O10" sqref="O10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="3" width="6.7109375" customWidth="1"/>
+    <col min="4" max="16" width="5.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="N1" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="O1" s="15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="9">
+        <f>SUM(D2:P2)</f>
+        <v>3320</v>
+      </c>
+      <c r="D2" s="3">
+        <f>SUMPRODUCT(D3:D36,$B$3:$B$36)</f>
+        <v>245</v>
+      </c>
+      <c r="E2" s="3">
+        <f>SUMPRODUCT(E3:E36,$B$3:$B$36)</f>
+        <v>504</v>
+      </c>
+      <c r="F2" s="3">
+        <f>SUMPRODUCT(F3:F36,$B$3:$B$36)</f>
+        <v>171</v>
+      </c>
+      <c r="G2" s="3">
+        <f>SUMPRODUCT(G3:G36,$B$3:$B$36)</f>
+        <v>195</v>
+      </c>
+      <c r="H2" s="3">
+        <f>SUMPRODUCT(H3:H36,$B$3:$B$36)</f>
+        <v>340</v>
+      </c>
+      <c r="I2" s="3">
+        <f>SUMPRODUCT(I3:I36,$B$3:$B$36)</f>
+        <v>395</v>
+      </c>
+      <c r="J2" s="3">
+        <f>SUMPRODUCT(J3:J36,$B$3:$B$36)</f>
+        <v>272</v>
+      </c>
+      <c r="K2" s="3">
+        <f>SUMPRODUCT(K3:K36,$B$3:$B$36)</f>
+        <v>510</v>
+      </c>
+      <c r="L2" s="3">
+        <f>SUMPRODUCT(L3:L36,$B$3:$B$36)</f>
+        <v>230</v>
+      </c>
+      <c r="M2" s="3">
+        <f>SUMPRODUCT(M3:M36,$B$3:$B$36)</f>
+        <v>83</v>
+      </c>
+      <c r="N2" s="3">
+        <f>SUMPRODUCT(N3:N36,$B$3:$B$36)</f>
+        <v>175</v>
+      </c>
+      <c r="O2" s="3">
+        <f>SUMPRODUCT(O3:O36,$B$3:$B$36)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" s="14">
+        <v>3</v>
+      </c>
+      <c r="C3" s="9">
+        <f t="shared" ref="C3:C19" si="0">SUM(D3:P3)</f>
+        <v>6</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3">
+        <v>6</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" s="14">
+        <v>12</v>
+      </c>
+      <c r="C4" s="9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3">
+        <v>4</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="14">
+        <v>12</v>
+      </c>
+      <c r="C5" s="9">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="E5" s="3">
+        <v>20</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="14">
+        <v>1</v>
+      </c>
+      <c r="C6" s="9">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="D6" s="3">
+        <v>6</v>
+      </c>
+      <c r="E6" s="3">
+        <v>21</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="14">
+        <v>3</v>
+      </c>
+      <c r="C7" s="9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3">
+        <v>9</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B8" s="14">
+        <v>5</v>
+      </c>
+      <c r="C8" s="9">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3">
+        <v>12</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="14">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9">
+        <f t="shared" si="0"/>
+        <v>1667</v>
+      </c>
+      <c r="D9" s="3">
+        <v>187</v>
+      </c>
+      <c r="E9" s="3">
+        <v>201</v>
+      </c>
+      <c r="F9" s="3">
+        <v>75</v>
+      </c>
+      <c r="G9" s="3">
+        <v>38</v>
+      </c>
+      <c r="H9" s="3">
+        <v>85</v>
+      </c>
+      <c r="I9" s="3">
+        <v>297</v>
+      </c>
+      <c r="J9" s="3">
+        <v>201</v>
+      </c>
+      <c r="K9" s="3">
+        <v>190</v>
+      </c>
+      <c r="L9" s="3">
+        <v>130</v>
+      </c>
+      <c r="M9" s="3">
+        <v>22</v>
+      </c>
+      <c r="N9" s="3">
+        <v>107</v>
+      </c>
+      <c r="O9" s="3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="14">
+        <v>1</v>
+      </c>
+      <c r="C10" s="9">
+        <f>SUM(D10:P10)</f>
+        <v>63</v>
+      </c>
+      <c r="D10" s="3">
+        <v>3</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3">
+        <v>9</v>
+      </c>
+      <c r="H10" s="3">
+        <v>13</v>
+      </c>
+      <c r="I10" s="3">
+        <v>8</v>
+      </c>
+      <c r="K10" s="3">
+        <v>19</v>
+      </c>
+      <c r="L10" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="14">
+        <v>1</v>
+      </c>
+      <c r="C11" s="9">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="D11" s="3">
+        <v>3</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3">
+        <v>25</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>148</v>
+      </c>
+      <c r="B12" s="14">
+        <v>4</v>
+      </c>
+      <c r="C12" s="9">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="O12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>175</v>
+      </c>
+      <c r="B13" s="14">
+        <v>5</v>
+      </c>
+      <c r="C13" s="9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="O13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>176</v>
+      </c>
+      <c r="B14" s="14">
+        <v>5</v>
+      </c>
+      <c r="C14" s="9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="O14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>174</v>
+      </c>
+      <c r="B15" s="14">
+        <v>2</v>
+      </c>
+      <c r="C15" s="9">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="O15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="14">
+        <v>2</v>
+      </c>
+      <c r="C16" s="9">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3">
+        <v>6</v>
+      </c>
+      <c r="G16" s="3">
+        <v>5</v>
+      </c>
+      <c r="H16" s="3">
+        <v>3</v>
+      </c>
+      <c r="I16" s="3">
+        <v>2</v>
+      </c>
+      <c r="J16" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="14">
+        <v>3</v>
+      </c>
+      <c r="C17" s="9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3">
+        <v>3</v>
+      </c>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>177</v>
+      </c>
+      <c r="B18" s="14">
+        <v>2</v>
+      </c>
+      <c r="C18" s="9">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3">
+        <v>12</v>
+      </c>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="14">
+        <v>2</v>
+      </c>
+      <c r="C19" s="9">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D19" s="3">
+        <v>3</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3">
+        <v>6</v>
+      </c>
+      <c r="I19" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" s="14">
+        <v>2</v>
+      </c>
+      <c r="C20" s="9">
+        <f>SUM(D20:P20)</f>
+        <v>14</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3">
+        <v>14</v>
+      </c>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="14">
+        <v>3</v>
+      </c>
+      <c r="C21" s="9">
+        <f>SUM(D21:P21)</f>
+        <v>6</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3">
+        <v>6</v>
+      </c>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="14">
+        <v>1</v>
+      </c>
+      <c r="C22" s="9">
+        <f>SUM(D22:P22)</f>
+        <v>65</v>
+      </c>
+      <c r="D22" s="3">
+        <v>12</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1</v>
+      </c>
+      <c r="F22" s="3">
+        <v>5</v>
+      </c>
+      <c r="G22" s="3">
+        <v>3</v>
+      </c>
+      <c r="H22" s="3">
+        <v>7</v>
+      </c>
+      <c r="I22" s="3">
+        <v>8</v>
+      </c>
+      <c r="J22" s="3">
+        <v>12</v>
+      </c>
+      <c r="K22" s="3">
+        <v>6</v>
+      </c>
+      <c r="L22">
+        <v>5</v>
+      </c>
+      <c r="M22" s="3">
+        <v>2</v>
+      </c>
+      <c r="N22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="14">
+        <v>1</v>
+      </c>
+      <c r="C23" s="9">
+        <f>SUM(D23:P23)</f>
+        <v>137</v>
+      </c>
+      <c r="D23" s="3">
+        <v>9</v>
+      </c>
+      <c r="E23" s="3">
+        <v>12</v>
+      </c>
+      <c r="F23" s="3">
+        <v>19</v>
+      </c>
+      <c r="G23" s="3">
+        <v>4</v>
+      </c>
+      <c r="H23" s="3">
+        <v>19</v>
+      </c>
+      <c r="I23" s="3">
+        <v>2</v>
+      </c>
+      <c r="J23" s="3">
+        <v>28</v>
+      </c>
+      <c r="K23" s="3">
+        <v>34</v>
+      </c>
+      <c r="L23" s="3">
+        <v>4</v>
+      </c>
+      <c r="M23" s="3">
+        <v>4</v>
+      </c>
+      <c r="N23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="14">
+        <v>1</v>
+      </c>
+      <c r="C24" s="9">
+        <f>SUM(D24:P24)</f>
+        <v>242</v>
+      </c>
+      <c r="D24" s="3">
+        <v>13</v>
+      </c>
+      <c r="E24" s="3">
+        <v>5</v>
+      </c>
+      <c r="F24" s="3">
+        <v>13</v>
+      </c>
+      <c r="G24" s="3">
+        <v>11</v>
+      </c>
+      <c r="H24" s="3">
+        <v>32</v>
+      </c>
+      <c r="I24" s="3">
+        <v>26</v>
+      </c>
+      <c r="J24" s="3">
+        <v>4</v>
+      </c>
+      <c r="K24">
+        <v>49</v>
+      </c>
+      <c r="L24" s="3">
+        <v>58</v>
+      </c>
+      <c r="M24">
+        <v>6</v>
+      </c>
+      <c r="N24">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="14">
+        <v>1</v>
+      </c>
+      <c r="C25" s="9">
+        <f>SUM(D25:P25)</f>
+        <v>148</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3">
+        <v>4</v>
+      </c>
+      <c r="G25" s="3">
+        <v>1</v>
+      </c>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3">
+        <v>16</v>
+      </c>
+      <c r="J25" s="3"/>
+      <c r="K25">
+        <v>120</v>
+      </c>
+      <c r="L25">
+        <v>6</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B26" s="14">
+        <v>1</v>
+      </c>
+      <c r="C26" s="9">
+        <f>SUM(D26:P26)</f>
+        <v>66</v>
+      </c>
+      <c r="D26" s="3">
+        <v>4</v>
+      </c>
+      <c r="E26" s="3">
+        <v>8</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3">
+        <v>4</v>
+      </c>
+      <c r="H26" s="3">
+        <v>38</v>
+      </c>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3">
+        <v>9</v>
+      </c>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3">
+        <v>3</v>
+      </c>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="14">
+        <v>1</v>
+      </c>
+      <c r="C27" s="9">
+        <f>SUM(D27:P27)</f>
+        <v>1</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3">
+        <v>1</v>
+      </c>
+      <c r="J27" s="3"/>
+      <c r="M27" s="3"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>154</v>
+      </c>
+      <c r="B28" s="14">
+        <v>1</v>
+      </c>
+      <c r="C28" s="9">
+        <f>SUM(D28:P28)</f>
+        <v>112</v>
+      </c>
+      <c r="D28" s="3">
+        <v>1</v>
+      </c>
+      <c r="E28" s="3">
+        <v>2</v>
+      </c>
+      <c r="F28" s="3">
+        <v>2</v>
+      </c>
+      <c r="H28" s="3">
+        <v>15</v>
+      </c>
+      <c r="I28" s="3">
+        <v>3</v>
+      </c>
+      <c r="J28" s="3">
+        <v>1</v>
+      </c>
+      <c r="K28" s="3">
+        <v>80</v>
+      </c>
+      <c r="L28" s="3">
+        <v>4</v>
+      </c>
+      <c r="M28">
+        <v>2</v>
+      </c>
+      <c r="N28" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>155</v>
+      </c>
+      <c r="B29" s="14">
+        <v>3</v>
+      </c>
+      <c r="C29" s="9">
+        <f>SUM(D29:P29)</f>
+        <v>22</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="H29" s="3">
+        <v>4</v>
+      </c>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3">
+        <v>14</v>
+      </c>
+      <c r="N29" s="3">
+        <v>4</v>
+      </c>
+      <c r="O29" s="3"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>156</v>
+      </c>
+      <c r="B30" s="14">
+        <v>1</v>
+      </c>
+      <c r="C30" s="9">
+        <f>SUM(D30:P30)</f>
+        <v>11</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="F30" s="3">
+        <v>4</v>
+      </c>
+      <c r="H30" s="3">
+        <v>3</v>
+      </c>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="M30">
+        <v>4</v>
+      </c>
+      <c r="N30" s="3"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>157</v>
+      </c>
+      <c r="B31" s="14">
+        <v>1</v>
+      </c>
+      <c r="C31" s="9">
+        <f>SUM(D31:P31)</f>
+        <v>29</v>
+      </c>
+      <c r="D31" s="3">
+        <v>1</v>
+      </c>
+      <c r="E31" s="3">
+        <v>1</v>
+      </c>
+      <c r="F31" s="3">
+        <v>1</v>
+      </c>
+      <c r="H31" s="3">
+        <v>2</v>
+      </c>
+      <c r="I31" s="3">
+        <v>1</v>
+      </c>
+      <c r="J31" s="3">
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="N31">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>158</v>
+      </c>
+      <c r="B32" s="14">
+        <v>1</v>
+      </c>
+      <c r="C32" s="9">
+        <f>SUM(D32:P32)</f>
+        <v>40</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>2</v>
+      </c>
+      <c r="I32">
+        <v>15</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>11</v>
+      </c>
+      <c r="L32">
+        <v>8</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>159</v>
+      </c>
+      <c r="B33" s="14">
+        <v>1</v>
+      </c>
+      <c r="C33" s="9">
+        <f>SUM(D33:P33)</f>
+        <v>8</v>
+      </c>
+      <c r="I33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I34">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>